<commit_message>
suppr slice identifier orga
Déjà définie dans fr.core 692bc0b403bdf29e07d674c0d3d5199aa3e84313
</commit_message>
<xml_diff>
--- a/sd-add-new-fr-core/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/sd-add-new-fr-core/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-03T08:07:04+00:00</t>
+    <t>2024-04-03T09:10:32+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -827,7 +827,7 @@
     <t>HealthcareService.providedBy</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://interopsante.org/fhir/StructureDefinition/FrOrganization|https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-organization)
+    <t xml:space="preserve">Reference(https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-organization|https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-organization)
 </t>
   </si>
   <si>
@@ -2550,7 +2550,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="138.9140625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="140.9453125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>